<commit_message>
Fixed categories in computer code modules
</commit_message>
<xml_diff>
--- a/DataChecklistModules.xlsx
+++ b/DataChecklistModules.xlsx
@@ -2161,6 +2161,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2973,8 +2974,8 @@
   <dimension ref="A1:F1050"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A283" sqref="A283"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>